<commit_message>
Added comments.  Updated an auto distance (it's a bit dependent on battery power).
</commit_message>
<xml_diff>
--- a/elegoo_robot/Arduino Pinout.xlsx
+++ b/elegoo_robot/Arduino Pinout.xlsx
@@ -1,13 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="150" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eric Gaudet</author>
+  </authors>
+  <commentList>
+    <comment ref="D15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Eric Gaudet:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Need to phyically disconnect this pin from the soldered IR circuitry.  Did this by using extention pins between the Arduino and the Elegoo I/O board and then disconnected D12 on the extention.  This saved me from unsoldering the IR stuff.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -199,47 +236,74 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF980000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF980000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFD9D9D9"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -247,7 +311,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -257,66 +321,46 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -327,11 +371,11 @@
     <xdr:ext cx="8582025" cy="6143625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -349,7 +393,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -539,23 +583,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="5.71"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +615,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -585,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -619,7 +666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -633,7 +680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -647,7 +694,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -661,7 +708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -675,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -689,7 +736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -703,7 +750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -717,7 +764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -731,7 +778,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -745,7 +792,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -759,7 +806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -773,10 +820,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -790,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -804,7 +851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -818,7 +865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -832,7 +879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -846,7 +893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -860,7 +907,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -873,11 +920,11 @@
       <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -890,11 +937,11 @@
       <c r="D26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -907,11 +954,11 @@
       <c r="D27" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -924,11 +971,11 @@
       <c r="D28" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -941,11 +988,11 @@
       <c r="D29" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -958,11 +1005,11 @@
       <c r="D30" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -975,11 +1022,11 @@
       <c r="D31" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -992,9 +1039,12 @@
       <c r="D32" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="16"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>